<commit_message>
2 samples for the same lib
</commit_message>
<xml_diff>
--- a/files/biosamples-and-sequencing.xlsx
+++ b/files/biosamples-and-sequencing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kad/projects/cog-uk/cog-uk.io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au3/Documents/code/covid19/cog-uk.io/website/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D98BB-A87D-6340-B5C1-048E10D3049C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AAFB04-D1C3-5C46-8772-BD7DE24A1FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2360" windowWidth="32100" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="2840" windowWidth="39840" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cog-uk-metadata-template_sample" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>adm1</t>
   </si>
@@ -248,7 +248,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1085,20 +1085,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:AD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="19" width="10.83203125" style="1"/>
+    <col min="1" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="20.6640625" style="1" customWidth="1"/>
+    <col min="18" max="19" width="10.83203125" style="1"/>
     <col min="20" max="20" width="18.5" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="23.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="24.5" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1202,12 +1204,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:16384">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:16384">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -1218,7 +1220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:16384">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -17625,7 +17627,7 @@
       <c r="XFC4"/>
       <c r="XFD4"/>
     </row>
-    <row r="5" spans="1:16384">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -34035,7 +34037,7 @@
       <c r="XFC5"/>
       <c r="XFD5"/>
     </row>
-    <row r="6" spans="1:16384">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -50443,7 +50445,7 @@
       <c r="XFC6"/>
       <c r="XFD6"/>
     </row>
-    <row r="7" spans="1:16384">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -66853,7 +66855,7 @@
       <c r="XFC7"/>
       <c r="XFD7"/>
     </row>
-    <row r="8" spans="1:16384">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -66872,8 +66874,44 @@
       <c r="I8" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="Q8" t="s">
+        <v>59</v>
+      </c>
+      <c r="R8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" t="s">
+        <v>61</v>
+      </c>
+      <c r="T8" t="s">
+        <v>62</v>
+      </c>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="9" spans="1:16384">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -66893,7 +66931,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:16384">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -66915,5 +66953,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>